<commit_message>
Actualizar conjunto de datos de infraestructura
</commit_message>
<xml_diff>
--- a/infraestructura/processed/infraestructura-corredores.xlsx
+++ b/infraestructura/processed/infraestructura-corredores.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
-    <t xml:space="preserve">Corredores Biológicos</t>
+    <t xml:space="preserve">Corredor</t>
   </si>
   <si>
     <t xml:space="preserve">Arbolados a lo largo de las autopistas</t>
@@ -100,10 +100,10 @@
     <t xml:space="preserve">Tiribí</t>
   </si>
   <si>
-    <t xml:space="preserve">Río Torres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">María Aguilar</t>
+    <t xml:space="preserve">Rí­o Torres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marí­a Aguilar</t>
   </si>
 </sst>
 </file>
@@ -299,10 +299,10 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.17"/>
@@ -313,7 +313,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.63"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +703,7 @@
         <v>37.827936</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -768,7 +768,7 @@
         <v>22.567248</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>